<commit_message>
handle section titles, non-ojs metadata, skipping non-doiable articles
</commit_message>
<xml_diff>
--- a/scenario_tocs.xlsx
+++ b/scenario_tocs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\xMeta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3B9BF1A-DCA9-4591-9E40-92A2F52C994E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C9F9681-7715-4B02-A3CB-928BA071DFF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3963" uniqueCount="1586">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3980" uniqueCount="1588">
   <si>
     <t>issue_url</t>
   </si>
@@ -4846,6 +4846,12 @@
   </si>
   <si>
     <t>Conference Items</t>
+  </si>
+  <si>
+    <t>Conference Item</t>
+  </si>
+  <si>
+    <t>n/a</t>
   </si>
 </sst>
 </file>
@@ -15570,7 +15576,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8F625CC-18F4-4775-BC1F-D600E757741E}">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -16609,10 +16615,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{684E9DB5-6864-4CCB-B516-676B6091924A}">
-  <dimension ref="A1:M17"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -16627,7 +16633,7 @@
     <col min="13" max="13" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>1537</v>
       </c>
@@ -16667,8 +16673,11 @@
       <c r="M1" t="s">
         <v>1545</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N1" t="s">
+        <v>1532</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>1560</v>
       </c>
@@ -16705,8 +16714,11 @@
       <c r="M2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>1555</v>
       </c>
@@ -16743,8 +16755,11 @@
       <c r="M3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N3" t="s">
+        <v>1534</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>1579</v>
       </c>
@@ -16781,8 +16796,11 @@
       <c r="M4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N4" t="s">
+        <v>1534</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>1556</v>
       </c>
@@ -16817,8 +16835,11 @@
       <c r="M5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N5" t="s">
+        <v>1586</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>1552</v>
       </c>
@@ -16853,8 +16874,11 @@
       <c r="M6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N6" t="s">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>1553</v>
       </c>
@@ -16891,8 +16915,11 @@
       <c r="M7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N7" t="s">
+        <v>1092</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>1558</v>
       </c>
@@ -16929,8 +16956,11 @@
       <c r="M8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N8" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>1551</v>
       </c>
@@ -16967,8 +16997,11 @@
       <c r="M9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N9" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>1559</v>
       </c>
@@ -17003,8 +17036,11 @@
       <c r="M10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N10" t="s">
+        <v>1534</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>1557</v>
       </c>
@@ -17041,8 +17077,11 @@
       <c r="M11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N11" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>1554</v>
       </c>
@@ -17077,8 +17116,11 @@
       <c r="M12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N12" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>1562</v>
       </c>
@@ -17115,8 +17157,11 @@
       <c r="M13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N13" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>1548</v>
       </c>
@@ -17153,8 +17198,11 @@
       <c r="M14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N14" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>1550</v>
       </c>
@@ -17189,8 +17237,11 @@
       <c r="M15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N15" t="s">
+        <v>1587</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>1549</v>
       </c>
@@ -17225,8 +17276,11 @@
       <c r="M16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N16" t="s">
+        <v>1587</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>1563</v>
       </c>
@@ -17262,6 +17316,9 @@
       </c>
       <c r="M17">
         <v>0</v>
+      </c>
+      <c r="N17" t="s">
+        <v>1587</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
handle page numbers, and better html parsing
</commit_message>
<xml_diff>
--- a/scenario_tocs.xlsx
+++ b/scenario_tocs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\xMeta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C9F9681-7715-4B02-A3CB-928BA071DFF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18F29878-7344-4A77-9D2C-0D7DE98F3838}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3980" uniqueCount="1588">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3987" uniqueCount="1595">
   <si>
     <t>issue_url</t>
   </si>
@@ -4656,9 +4656,6 @@
     <t>Practitioners' Voices</t>
   </si>
   <si>
-    <t>Conference items</t>
-  </si>
-  <si>
     <t>Terminology Matters</t>
   </si>
   <si>
@@ -4852,6 +4849,30 @@
   </si>
   <si>
     <t>n/a</t>
+  </si>
+  <si>
+    <t>Rezensionen</t>
+  </si>
+  <si>
+    <t>Conference Announcements</t>
+  </si>
+  <si>
+    <t>Konferenzankündigungen</t>
+  </si>
+  <si>
+    <t>Conference Contributions</t>
+  </si>
+  <si>
+    <t>Konferenzbeiträge</t>
+  </si>
+  <si>
+    <t>Texts around Theater</t>
+  </si>
+  <si>
+    <t>Terminology</t>
+  </si>
+  <si>
+    <t>Terminologie</t>
   </si>
 </sst>
 </file>
@@ -5266,7 +5287,7 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="F2" t="s">
         <v>15</v>
@@ -5295,7 +5316,7 @@
         <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="F3" t="s">
         <v>21</v>
@@ -5596,7 +5617,7 @@
         <v>14</v>
       </c>
       <c r="D14" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="F14" t="s">
         <v>15</v>
@@ -5622,7 +5643,7 @@
         <v>20</v>
       </c>
       <c r="D15" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="F15" t="s">
         <v>79</v>
@@ -5897,7 +5918,7 @@
         <v>14</v>
       </c>
       <c r="D25" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="F25" t="s">
         <v>15</v>
@@ -5926,7 +5947,7 @@
         <v>20</v>
       </c>
       <c r="D26" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="F26" t="s">
         <v>79</v>
@@ -6207,7 +6228,7 @@
         <v>14</v>
       </c>
       <c r="D36" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="F36" t="s">
         <v>15</v>
@@ -6233,7 +6254,7 @@
         <v>20</v>
       </c>
       <c r="D37" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="F37" t="s">
         <v>79</v>
@@ -6537,7 +6558,7 @@
         <v>14</v>
       </c>
       <c r="D48" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="F48" t="s">
         <v>15</v>
@@ -6563,7 +6584,7 @@
         <v>20</v>
       </c>
       <c r="D49" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="F49" t="s">
         <v>79</v>
@@ -6870,7 +6891,7 @@
         <v>14</v>
       </c>
       <c r="D60" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="F60" t="s">
         <v>15</v>
@@ -6896,7 +6917,7 @@
         <v>20</v>
       </c>
       <c r="D61" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="F61" t="s">
         <v>79</v>
@@ -7168,7 +7189,7 @@
         <v>14</v>
       </c>
       <c r="D71" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="F71" t="s">
         <v>15</v>
@@ -7194,7 +7215,7 @@
         <v>20</v>
       </c>
       <c r="D72" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="F72" t="s">
         <v>21</v>
@@ -7431,7 +7452,7 @@
         <v>14</v>
       </c>
       <c r="D81" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="F81" t="s">
         <v>15</v>
@@ -7457,7 +7478,7 @@
         <v>20</v>
       </c>
       <c r="D82" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="F82" t="s">
         <v>79</v>
@@ -7706,7 +7727,7 @@
         <v>14</v>
       </c>
       <c r="D91" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="F91" t="s">
         <v>15</v>
@@ -7732,7 +7753,7 @@
         <v>20</v>
       </c>
       <c r="D92" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="F92" t="s">
         <v>79</v>
@@ -8143,7 +8164,7 @@
         <v>14</v>
       </c>
       <c r="D107" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="F107" t="s">
         <v>15</v>
@@ -8169,7 +8190,7 @@
         <v>20</v>
       </c>
       <c r="D108" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="F108" t="s">
         <v>79</v>
@@ -8551,7 +8572,7 @@
         <v>14</v>
       </c>
       <c r="D122" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="F122" t="s">
         <v>15</v>
@@ -8577,7 +8598,7 @@
         <v>20</v>
       </c>
       <c r="D123" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="F123" t="s">
         <v>79</v>
@@ -8933,7 +8954,7 @@
         <v>14</v>
       </c>
       <c r="D136" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="F136" t="s">
         <v>15</v>
@@ -8959,7 +8980,7 @@
         <v>20</v>
       </c>
       <c r="D137" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="F137" t="s">
         <v>21</v>
@@ -9300,7 +9321,7 @@
         <v>14</v>
       </c>
       <c r="D150" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="F150" t="s">
         <v>15</v>
@@ -9326,7 +9347,7 @@
         <v>20</v>
       </c>
       <c r="D151" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="F151" t="s">
         <v>79</v>
@@ -9723,7 +9744,7 @@
         <v>14</v>
       </c>
       <c r="D165" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="F165" t="s">
         <v>15</v>
@@ -9749,7 +9770,7 @@
         <v>20</v>
       </c>
       <c r="D166" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="F166" t="s">
         <v>79</v>
@@ -10134,7 +10155,7 @@
         <v>14</v>
       </c>
       <c r="D180" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="F180" t="s">
         <v>15</v>
@@ -10160,7 +10181,7 @@
         <v>20</v>
       </c>
       <c r="D181" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="F181" t="s">
         <v>79</v>
@@ -10461,7 +10482,7 @@
         <v>14</v>
       </c>
       <c r="D192" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="F192" t="s">
         <v>15</v>
@@ -10487,7 +10508,7 @@
         <v>20</v>
       </c>
       <c r="D193" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="F193" t="s">
         <v>21</v>
@@ -10904,7 +10925,7 @@
         <v>845</v>
       </c>
       <c r="D208" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="F208" t="s">
         <v>15</v>
@@ -10930,7 +10951,7 @@
         <v>848</v>
       </c>
       <c r="D209" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="F209" t="s">
         <v>79</v>
@@ -11283,7 +11304,7 @@
         <v>14</v>
       </c>
       <c r="D222" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="F222" t="s">
         <v>26</v>
@@ -11309,7 +11330,7 @@
         <v>20</v>
       </c>
       <c r="D223" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="F223" t="s">
         <v>89</v>
@@ -11578,7 +11599,7 @@
         <v>14</v>
       </c>
       <c r="D233" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="F233" t="s">
         <v>15</v>
@@ -11604,7 +11625,7 @@
         <v>20</v>
       </c>
       <c r="D234" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="F234" t="s">
         <v>79</v>
@@ -12015,7 +12036,7 @@
         <v>14</v>
       </c>
       <c r="D249" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="F249" t="s">
         <v>15</v>
@@ -12041,7 +12062,7 @@
         <v>20</v>
       </c>
       <c r="D250" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="F250" t="s">
         <v>79</v>
@@ -12516,7 +12537,7 @@
         <v>14</v>
       </c>
       <c r="D267" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="F267" t="s">
         <v>15</v>
@@ -12542,7 +12563,7 @@
         <v>20</v>
       </c>
       <c r="D268" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="F268" t="s">
         <v>21</v>
@@ -12924,7 +12945,7 @@
         <v>14</v>
       </c>
       <c r="D282" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="F282" t="s">
         <v>15</v>
@@ -12950,7 +12971,7 @@
         <v>20</v>
       </c>
       <c r="D283" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="F283" t="s">
         <v>79</v>
@@ -13228,7 +13249,7 @@
         <v>14</v>
       </c>
       <c r="D293" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="F293" t="s">
         <v>15</v>
@@ -13254,7 +13275,7 @@
         <v>20</v>
       </c>
       <c r="D294" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="F294" t="s">
         <v>79</v>
@@ -13610,7 +13631,7 @@
         <v>14</v>
       </c>
       <c r="D307" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="F307" t="s">
         <v>15</v>
@@ -13636,7 +13657,7 @@
         <v>20</v>
       </c>
       <c r="D308" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="F308" t="s">
         <v>79</v>
@@ -14366,7 +14387,7 @@
         <v>1344</v>
       </c>
       <c r="D334" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="F334" t="s">
         <v>15</v>
@@ -14803,7 +14824,7 @@
         <v>1344</v>
       </c>
       <c r="D350" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="F350" t="s">
         <v>15</v>
@@ -15211,7 +15232,7 @@
         <v>1463</v>
       </c>
       <c r="D365" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="F365" t="s">
         <v>15</v>
@@ -15576,8 +15597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8F625CC-18F4-4775-BC1F-D600E757741E}">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -15597,16 +15618,16 @@
         <v>1514</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>1534</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>1535</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>1536</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>1537</v>
-      </c>
       <c r="F1" s="3" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
@@ -15620,10 +15641,10 @@
         <v>1516</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>1562</v>
+        <v>1561</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>772</v>
@@ -15637,21 +15658,21 @@
         <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>1528</v>
+        <v>1527</v>
       </c>
       <c r="D3" t="s">
         <v>564</v>
       </c>
       <c r="E3" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
       <c r="F3" t="s">
-        <v>1533</v>
+        <v>1532</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="B4" s="2">
         <v>51</v>
@@ -15663,10 +15684,10 @@
         <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>1560</v>
+        <v>1559</v>
       </c>
       <c r="F4" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
@@ -15680,10 +15701,10 @@
         <v>1515</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>66</v>
+        <v>1587</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
       <c r="F5" t="s">
         <v>212</v>
@@ -15699,11 +15720,14 @@
       <c r="C6" t="s">
         <v>996</v>
       </c>
+      <c r="D6" t="s">
+        <v>996</v>
+      </c>
       <c r="E6" t="s">
-        <v>1549</v>
+        <v>1548</v>
       </c>
       <c r="F6" t="s">
-        <v>1533</v>
+        <v>1532</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
@@ -15720,10 +15744,10 @@
         <v>1221</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
       <c r="F7" t="s">
-        <v>1533</v>
+        <v>1532</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
@@ -15737,10 +15761,10 @@
         <v>1516</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>1562</v>
+        <v>1561</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>772</v>
@@ -15757,10 +15781,10 @@
         <v>1516</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>1562</v>
+        <v>1561</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>772</v>
@@ -15777,10 +15801,10 @@
         <v>1516</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>1562</v>
+        <v>1561</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>772</v>
@@ -15796,11 +15820,14 @@
       <c r="C11" t="s">
         <v>1518</v>
       </c>
+      <c r="D11" s="1" t="s">
+        <v>1518</v>
+      </c>
       <c r="E11" t="s">
-        <v>1552</v>
+        <v>1551</v>
       </c>
       <c r="F11" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
@@ -15814,10 +15841,10 @@
         <v>1517</v>
       </c>
       <c r="D12" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
       <c r="E12" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
       <c r="F12" t="s">
         <v>1092</v>
@@ -15834,10 +15861,10 @@
         <v>1516</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>1562</v>
+        <v>1561</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>772</v>
@@ -15853,8 +15880,11 @@
       <c r="C14" t="s">
         <v>1519</v>
       </c>
+      <c r="D14" s="1" t="s">
+        <v>1519</v>
+      </c>
       <c r="E14" t="s">
-        <v>1554</v>
+        <v>1553</v>
       </c>
       <c r="F14" t="s">
         <v>489</v>
@@ -15868,16 +15898,16 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>1336</v>
+        <v>1588</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>1221</v>
+        <v>1589</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
       <c r="F15" t="s">
-        <v>1533</v>
+        <v>1532</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
@@ -15891,10 +15921,10 @@
         <v>1516</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>1562</v>
+        <v>1561</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>772</v>
@@ -15908,10 +15938,13 @@
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>1522</v>
+        <v>1590</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>1591</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
       <c r="F17" t="s">
         <v>1520</v>
@@ -15928,10 +15961,10 @@
         <v>1516</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>1562</v>
+        <v>1561</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>772</v>
@@ -15945,10 +15978,13 @@
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>1522</v>
+        <v>1590</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>1591</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
       <c r="F19" t="s">
         <v>1520</v>
@@ -15968,10 +16004,10 @@
         <v>808</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>1557</v>
+        <v>1556</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
@@ -15985,10 +16021,10 @@
         <v>1516</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>1562</v>
+        <v>1561</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>772</v>
@@ -16005,10 +16041,10 @@
         <v>1515</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>66</v>
+        <v>1587</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
       <c r="F22" t="s">
         <v>212</v>
@@ -16025,10 +16061,10 @@
         <v>1515</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>66</v>
+        <v>1587</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
       <c r="F23" t="s">
         <v>212</v>
@@ -16042,16 +16078,16 @@
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>1517</v>
+        <v>1590</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>1531</v>
+        <v>1591</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
       <c r="F24" t="s">
-        <v>1092</v>
+        <v>1520</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
@@ -16062,16 +16098,16 @@
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>1517</v>
+        <v>1590</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>1531</v>
+        <v>1591</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
       <c r="F25" t="s">
-        <v>1092</v>
+        <v>1520</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
@@ -16082,10 +16118,13 @@
         <v>3</v>
       </c>
       <c r="C26" t="s">
-        <v>1522</v>
+        <v>1590</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>1591</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
       <c r="F26" t="s">
         <v>1520</v>
@@ -16099,16 +16138,16 @@
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>1521</v>
+        <v>504</v>
       </c>
       <c r="D27" t="s">
-        <v>1530</v>
+        <v>808</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="F27" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
@@ -16119,16 +16158,16 @@
         <v>1</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>980</v>
+        <v>504</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>975</v>
+        <v>808</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
@@ -16139,16 +16178,16 @@
         <v>2</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>980</v>
+        <v>504</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>975</v>
+        <v>808</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
@@ -16162,10 +16201,10 @@
         <v>1516</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>1562</v>
+        <v>1561</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>772</v>
@@ -16179,16 +16218,16 @@
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>1014</v>
+        <v>1592</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>1584</v>
+        <v>450</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="F31" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
@@ -16199,16 +16238,16 @@
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>1014</v>
+        <v>1592</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>1584</v>
+        <v>450</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="F32" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.45">
@@ -16219,16 +16258,16 @@
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>1014</v>
+        <v>1592</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>1584</v>
+        <v>450</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="F33" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.45">
@@ -16239,16 +16278,16 @@
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>1014</v>
+        <v>1592</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>1584</v>
+        <v>450</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="F34" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.45">
@@ -16259,16 +16298,16 @@
         <v>5</v>
       </c>
       <c r="C35" t="s">
-        <v>1014</v>
+        <v>1592</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>1584</v>
+        <v>450</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="F35" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
@@ -16279,16 +16318,16 @@
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>1014</v>
+        <v>1592</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>1584</v>
+        <v>450</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="F36" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
@@ -16299,16 +16338,16 @@
         <v>5</v>
       </c>
       <c r="C37" t="s">
-        <v>1014</v>
+        <v>1592</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>1584</v>
+        <v>450</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="F37" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
@@ -16319,16 +16358,16 @@
         <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>1014</v>
+        <v>1592</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>1584</v>
+        <v>450</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="F38" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.45">
@@ -16339,14 +16378,16 @@
         <v>1</v>
       </c>
       <c r="C39" t="s">
-        <v>1523</v>
-      </c>
-      <c r="D39" s="1"/>
+        <v>1593</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>1594</v>
+      </c>
       <c r="E39" s="1" t="s">
-        <v>1559</v>
+        <v>1558</v>
       </c>
       <c r="F39" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.45">
@@ -16357,16 +16398,16 @@
         <v>2</v>
       </c>
       <c r="C40" t="s">
-        <v>1014</v>
+        <v>1592</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>1584</v>
+        <v>450</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="F40" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.45">
@@ -16377,16 +16418,16 @@
         <v>2</v>
       </c>
       <c r="C41" t="s">
-        <v>1014</v>
+        <v>1592</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>1584</v>
+        <v>450</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="F41" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.45">
@@ -16397,16 +16438,16 @@
         <v>1</v>
       </c>
       <c r="C42" t="s">
-        <v>1014</v>
+        <v>1592</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>1584</v>
+        <v>450</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="F42" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.45">
@@ -16417,16 +16458,16 @@
         <v>2</v>
       </c>
       <c r="C43" t="s">
-        <v>1014</v>
+        <v>1592</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>1584</v>
+        <v>450</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="F43" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.45">
@@ -16437,16 +16478,16 @@
         <v>1</v>
       </c>
       <c r="C44" t="s">
-        <v>1014</v>
+        <v>1592</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>1584</v>
+        <v>450</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="F44" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.45">
@@ -16457,16 +16498,16 @@
         <v>1</v>
       </c>
       <c r="C45" t="s">
-        <v>1014</v>
+        <v>1592</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>1584</v>
+        <v>450</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="F45" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.45">
@@ -16477,16 +16518,16 @@
         <v>1</v>
       </c>
       <c r="C46" t="s">
-        <v>1014</v>
+        <v>1592</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>1584</v>
+        <v>450</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="F46" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.45">
@@ -16497,16 +16538,16 @@
         <v>6</v>
       </c>
       <c r="C47" t="s">
-        <v>1014</v>
+        <v>1592</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>1584</v>
+        <v>450</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="F47" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.45">
@@ -16523,10 +16564,10 @@
         <v>808</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>1557</v>
+        <v>1556</v>
       </c>
       <c r="F48" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.45">
@@ -16543,10 +16584,10 @@
         <v>808</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>1557</v>
+        <v>1556</v>
       </c>
       <c r="F49" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.45">
@@ -16557,16 +16598,16 @@
         <v>4</v>
       </c>
       <c r="C50" t="s">
-        <v>1516</v>
+        <v>1590</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>1529</v>
+        <v>1591</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>1562</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>772</v>
+        <v>1561</v>
+      </c>
+      <c r="F50" t="s">
+        <v>1520</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.45">
@@ -16577,33 +16618,33 @@
         <v>2</v>
       </c>
       <c r="C51" t="s">
-        <v>1516</v>
+        <v>1590</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>1529</v>
+        <v>1591</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>1562</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>772</v>
+        <v>1561</v>
+      </c>
+      <c r="F51" t="s">
+        <v>1520</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52" s="1" t="s">
+        <v>1579</v>
+      </c>
+      <c r="C52" t="s">
         <v>1580</v>
       </c>
-      <c r="C52" t="s">
+      <c r="D52" s="1" t="s">
         <v>1581</v>
       </c>
-      <c r="D52" s="1" t="s">
-        <v>1582</v>
-      </c>
       <c r="E52" s="1" t="s">
-        <v>1579</v>
+        <v>1578</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
     </row>
   </sheetData>
@@ -16617,7 +16658,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{684E9DB5-6864-4CCB-B516-676B6091924A}">
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
@@ -16635,51 +16676,51 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>1536</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1534</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1535</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1545</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1546</v>
+      </c>
+      <c r="F1" t="s">
         <v>1537</v>
       </c>
-      <c r="B1" t="s">
-        <v>1535</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1536</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1546</v>
-      </c>
-      <c r="E1" t="s">
-        <v>1547</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>1538</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>1539</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>1540</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>1541</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>1542</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>1543</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>1544</v>
       </c>
-      <c r="M1" t="s">
-        <v>1545</v>
-      </c>
       <c r="N1" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
-        <v>1560</v>
+        <v>1559</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>14</v>
@@ -16688,7 +16729,7 @@
         <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -16720,16 +16761,16 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>1014</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1584</v>
+        <v>1583</v>
       </c>
       <c r="D3" t="s">
-        <v>1576</v>
+        <v>1575</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -16756,21 +16797,21 @@
         <v>0</v>
       </c>
       <c r="N3" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
-        <v>1579</v>
+        <v>1578</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>1580</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>1581</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" t="s">
         <v>1582</v>
-      </c>
-      <c r="D4" t="s">
-        <v>1583</v>
       </c>
       <c r="F4">
         <v>2</v>
@@ -16797,19 +16838,19 @@
         <v>0</v>
       </c>
       <c r="N4" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>1585</v>
+        <v>1584</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
       <c r="F5">
         <v>3</v>
@@ -16836,19 +16877,19 @@
         <v>0</v>
       </c>
       <c r="N5" t="s">
-        <v>1586</v>
+        <v>1585</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
-        <v>1552</v>
+        <v>1551</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>1518</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" t="s">
-        <v>1568</v>
+        <v>1567</v>
       </c>
       <c r="F6">
         <v>4</v>
@@ -16880,16 +16921,16 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>1517</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
       <c r="D7" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
       <c r="F7">
         <v>5</v>
@@ -16921,16 +16962,16 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>1521</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1530</v>
+        <v>1529</v>
       </c>
       <c r="D8" t="s">
-        <v>1572</v>
+        <v>1571</v>
       </c>
       <c r="F8">
         <v>6</v>
@@ -16962,7 +17003,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>980</v>
@@ -16971,7 +17012,7 @@
         <v>975</v>
       </c>
       <c r="D9" t="s">
-        <v>1575</v>
+        <v>1574</v>
       </c>
       <c r="F9">
         <v>9</v>
@@ -17003,14 +17044,14 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
-        <v>1559</v>
+        <v>1558</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" t="s">
-        <v>1577</v>
+        <v>1576</v>
       </c>
       <c r="F10">
         <v>10</v>
@@ -17037,12 +17078,12 @@
         <v>0</v>
       </c>
       <c r="N10" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
-        <v>1557</v>
+        <v>1556</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>504</v>
@@ -17051,7 +17092,7 @@
         <v>808</v>
       </c>
       <c r="D11" t="s">
-        <v>1578</v>
+        <v>1577</v>
       </c>
       <c r="F11">
         <v>11</v>
@@ -17083,14 +17124,14 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
-        <v>1554</v>
+        <v>1553</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>1519</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" t="s">
-        <v>1571</v>
+        <v>1570</v>
       </c>
       <c r="F12">
         <v>12</v>
@@ -17122,16 +17163,16 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
-        <v>1562</v>
+        <v>1561</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>1516</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
       <c r="D13" t="s">
-        <v>1573</v>
+        <v>1572</v>
       </c>
       <c r="F13">
         <v>7</v>
@@ -17163,7 +17204,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>1515</v>
@@ -17172,7 +17213,7 @@
         <v>66</v>
       </c>
       <c r="D14" t="s">
-        <v>1574</v>
+        <v>1573</v>
       </c>
       <c r="F14">
         <v>8</v>
@@ -17204,14 +17245,14 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>1336</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
       <c r="F15">
         <v>13</v>
@@ -17238,19 +17279,19 @@
         <v>0</v>
       </c>
       <c r="N15" t="s">
-        <v>1587</v>
+        <v>1586</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
-        <v>1549</v>
+        <v>1548</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>996</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
       <c r="F16">
         <v>14</v>
@@ -17277,21 +17318,21 @@
         <v>0</v>
       </c>
       <c r="N16" t="s">
-        <v>1587</v>
+        <v>1586</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>1528</v>
+        <v>1527</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>564</v>
       </c>
       <c r="D17" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
       <c r="F17">
         <v>15</v>
@@ -17318,7 +17359,7 @@
         <v>0</v>
       </c>
       <c r="N17" t="s">
-        <v>1587</v>
+        <v>1586</v>
       </c>
     </row>
   </sheetData>
@@ -17342,13 +17383,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>1524</v>
+        <v>1523</v>
       </c>
       <c r="B1" t="s">
         <v>1514</v>
       </c>
       <c r="C1" t="s">
-        <v>1525</v>
+        <v>1524</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
@@ -17359,7 +17400,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
@@ -17370,7 +17411,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
@@ -17381,7 +17422,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
@@ -17392,7 +17433,7 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
@@ -17403,7 +17444,7 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
@@ -17414,7 +17455,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
@@ -17425,7 +17466,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
@@ -17436,7 +17477,7 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
@@ -17447,7 +17488,7 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
@@ -17458,7 +17499,7 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
@@ -17469,7 +17510,7 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
@@ -17480,7 +17521,7 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
@@ -17491,7 +17532,7 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
@@ -17502,7 +17543,7 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.45">
@@ -17513,7 +17554,7 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.45">
@@ -17524,7 +17565,7 @@
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.45">
@@ -17535,7 +17576,7 @@
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
@@ -17546,7 +17587,7 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.45">
@@ -17557,7 +17598,7 @@
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.45">
@@ -17568,7 +17609,7 @@
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.45">
@@ -17579,7 +17620,7 @@
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.45">
@@ -17590,7 +17631,7 @@
         <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.45">
@@ -17601,7 +17642,7 @@
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.45">
@@ -17612,7 +17653,7 @@
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.45">
@@ -17623,7 +17664,7 @@
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.45">
@@ -17634,7 +17675,7 @@
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.45">
@@ -17645,7 +17686,7 @@
         <v>2</v>
       </c>
       <c r="C28" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.45">
@@ -17656,7 +17697,7 @@
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.45">
@@ -17667,7 +17708,7 @@
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.45">
@@ -17678,7 +17719,7 @@
         <v>2</v>
       </c>
       <c r="C31" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.45">
@@ -17689,7 +17730,7 @@
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.45">
@@ -17700,7 +17741,7 @@
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.45">
@@ -17711,7 +17752,7 @@
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.45">
@@ -17722,7 +17763,7 @@
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.45">
@@ -17733,7 +17774,7 @@
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.45">
@@ -17744,7 +17785,7 @@
         <v>2</v>
       </c>
       <c r="C37" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.45">
@@ -17755,7 +17796,7 @@
         <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.45">
@@ -17766,7 +17807,7 @@
         <v>1</v>
       </c>
       <c r="C39" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.45">
@@ -17777,7 +17818,7 @@
         <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.45">
@@ -17788,7 +17829,7 @@
         <v>3</v>
       </c>
       <c r="C41" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.45">
@@ -17799,7 +17840,7 @@
         <v>4</v>
       </c>
       <c r="C42" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.45">
@@ -17810,7 +17851,7 @@
         <v>1</v>
       </c>
       <c r="C43" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.45">
@@ -17821,7 +17862,7 @@
         <v>1</v>
       </c>
       <c r="C44" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.45">
@@ -17832,7 +17873,7 @@
         <v>1</v>
       </c>
       <c r="C45" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.45">
@@ -17843,7 +17884,7 @@
         <v>1</v>
       </c>
       <c r="C46" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.45">
@@ -17854,7 +17895,7 @@
         <v>1</v>
       </c>
       <c r="C47" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.45">
@@ -17865,7 +17906,7 @@
         <v>1</v>
       </c>
       <c r="C48" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.45">
@@ -17876,7 +17917,7 @@
         <v>1</v>
       </c>
       <c r="C49" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.45">
@@ -17887,7 +17928,7 @@
         <v>1</v>
       </c>
       <c r="C50" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.45">
@@ -17898,7 +17939,7 @@
         <v>1</v>
       </c>
       <c r="C51" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.45">
@@ -17909,7 +17950,7 @@
         <v>2</v>
       </c>
       <c r="C52" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.45">
@@ -17920,7 +17961,7 @@
         <v>1</v>
       </c>
       <c r="C53" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.45">
@@ -17931,7 +17972,7 @@
         <v>1</v>
       </c>
       <c r="C54" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.45">
@@ -17942,7 +17983,7 @@
         <v>2</v>
       </c>
       <c r="C55" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.45">
@@ -17953,7 +17994,7 @@
         <v>1</v>
       </c>
       <c r="C56" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.45">
@@ -17964,7 +18005,7 @@
         <v>1</v>
       </c>
       <c r="C57" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.45">
@@ -17975,7 +18016,7 @@
         <v>1</v>
       </c>
       <c r="C58" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.45">
@@ -17986,7 +18027,7 @@
         <v>1</v>
       </c>
       <c r="C59" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.45">
@@ -17997,7 +18038,7 @@
         <v>3</v>
       </c>
       <c r="C60" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.45">
@@ -18008,7 +18049,7 @@
         <v>1</v>
       </c>
       <c r="C61" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.45">
@@ -18019,7 +18060,7 @@
         <v>1</v>
       </c>
       <c r="C62" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.45">
@@ -18030,7 +18071,7 @@
         <v>1</v>
       </c>
       <c r="C63" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.45">
@@ -18041,7 +18082,7 @@
         <v>2</v>
       </c>
       <c r="C64" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.45">
@@ -18052,7 +18093,7 @@
         <v>1</v>
       </c>
       <c r="C65" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.45">
@@ -18063,7 +18104,7 @@
         <v>1</v>
       </c>
       <c r="C66" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.45">
@@ -18074,7 +18115,7 @@
         <v>1</v>
       </c>
       <c r="C67" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.45">
@@ -18085,7 +18126,7 @@
         <v>4</v>
       </c>
       <c r="C68" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.45">
@@ -18096,7 +18137,7 @@
         <v>2</v>
       </c>
       <c r="C69" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.45">
@@ -18107,7 +18148,7 @@
         <v>3</v>
       </c>
       <c r="C70" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.45">
@@ -18118,7 +18159,7 @@
         <v>1</v>
       </c>
       <c r="C71" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.45">
@@ -18129,7 +18170,7 @@
         <v>1</v>
       </c>
       <c r="C72" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.45">
@@ -18140,7 +18181,7 @@
         <v>1</v>
       </c>
       <c r="C73" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.45">
@@ -18151,7 +18192,7 @@
         <v>1</v>
       </c>
       <c r="C74" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.45">
@@ -18162,7 +18203,7 @@
         <v>3</v>
       </c>
       <c r="C75" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.45">
@@ -18173,7 +18214,7 @@
         <v>1</v>
       </c>
       <c r="C76" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.45">
@@ -18184,7 +18225,7 @@
         <v>1</v>
       </c>
       <c r="C77" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.45">
@@ -18195,7 +18236,7 @@
         <v>1</v>
       </c>
       <c r="C78" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.45">
@@ -18206,7 +18247,7 @@
         <v>1</v>
       </c>
       <c r="C79" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.45">
@@ -18217,7 +18258,7 @@
         <v>1</v>
       </c>
       <c r="C80" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.45">
@@ -18228,7 +18269,7 @@
         <v>1</v>
       </c>
       <c r="C81" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.45">
@@ -18239,7 +18280,7 @@
         <v>1</v>
       </c>
       <c r="C82" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.45">
@@ -18250,7 +18291,7 @@
         <v>1</v>
       </c>
       <c r="C83" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.45">
@@ -18261,7 +18302,7 @@
         <v>1</v>
       </c>
       <c r="C84" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.45">
@@ -18272,7 +18313,7 @@
         <v>4</v>
       </c>
       <c r="C85" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.45">
@@ -18283,7 +18324,7 @@
         <v>1</v>
       </c>
       <c r="C86" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.45">
@@ -18294,7 +18335,7 @@
         <v>3</v>
       </c>
       <c r="C87" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.45">
@@ -18305,7 +18346,7 @@
         <v>1</v>
       </c>
       <c r="C88" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.45">
@@ -18316,7 +18357,7 @@
         <v>2</v>
       </c>
       <c r="C89" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.45">
@@ -18327,7 +18368,7 @@
         <v>1</v>
       </c>
       <c r="C90" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.45">
@@ -18338,7 +18379,7 @@
         <v>1</v>
       </c>
       <c r="C91" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.45">
@@ -18349,7 +18390,7 @@
         <v>2</v>
       </c>
       <c r="C92" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.45">
@@ -18360,7 +18401,7 @@
         <v>1</v>
       </c>
       <c r="C93" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.45">
@@ -18371,7 +18412,7 @@
         <v>2</v>
       </c>
       <c r="C94" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.45">
@@ -18382,7 +18423,7 @@
         <v>1</v>
       </c>
       <c r="C95" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.45">
@@ -18393,7 +18434,7 @@
         <v>1</v>
       </c>
       <c r="C96" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.45">
@@ -18404,7 +18445,7 @@
         <v>1</v>
       </c>
       <c r="C97" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.45">
@@ -18415,7 +18456,7 @@
         <v>1</v>
       </c>
       <c r="C98" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.45">
@@ -18426,7 +18467,7 @@
         <v>1</v>
       </c>
       <c r="C99" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.45">
@@ -18437,7 +18478,7 @@
         <v>1</v>
       </c>
       <c r="C100" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.45">
@@ -18448,7 +18489,7 @@
         <v>1</v>
       </c>
       <c r="C101" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.45">
@@ -18459,7 +18500,7 @@
         <v>2</v>
       </c>
       <c r="C102" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.45">
@@ -18470,7 +18511,7 @@
         <v>1</v>
       </c>
       <c r="C103" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.45">
@@ -18481,7 +18522,7 @@
         <v>2</v>
       </c>
       <c r="C104" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.45">
@@ -18492,7 +18533,7 @@
         <v>2</v>
       </c>
       <c r="C105" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.45">
@@ -18503,7 +18544,7 @@
         <v>1</v>
       </c>
       <c r="C106" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.45">
@@ -18514,7 +18555,7 @@
         <v>2</v>
       </c>
       <c r="C107" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.45">
@@ -18525,7 +18566,7 @@
         <v>1</v>
       </c>
       <c r="C108" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.45">
@@ -18536,7 +18577,7 @@
         <v>1</v>
       </c>
       <c r="C109" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.45">
@@ -18547,7 +18588,7 @@
         <v>1</v>
       </c>
       <c r="C110" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.45">
@@ -18558,7 +18599,7 @@
         <v>1</v>
       </c>
       <c r="C111" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.45">
@@ -18569,7 +18610,7 @@
         <v>1</v>
       </c>
       <c r="C112" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.45">
@@ -18580,7 +18621,7 @@
         <v>1</v>
       </c>
       <c r="C113" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.45">
@@ -18591,7 +18632,7 @@
         <v>1</v>
       </c>
       <c r="C114" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.45">
@@ -18602,7 +18643,7 @@
         <v>1</v>
       </c>
       <c r="C115" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.45">
@@ -18613,7 +18654,7 @@
         <v>1</v>
       </c>
       <c r="C116" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.45">
@@ -18624,7 +18665,7 @@
         <v>2</v>
       </c>
       <c r="C117" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.45">
@@ -18635,7 +18676,7 @@
         <v>1</v>
       </c>
       <c r="C118" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.45">
@@ -18646,7 +18687,7 @@
         <v>1</v>
       </c>
       <c r="C119" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.45">
@@ -18657,7 +18698,7 @@
         <v>1</v>
       </c>
       <c r="C120" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.45">
@@ -18668,7 +18709,7 @@
         <v>1</v>
       </c>
       <c r="C121" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.45">
@@ -18679,7 +18720,7 @@
         <v>2</v>
       </c>
       <c r="C122" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.45">
@@ -18690,7 +18731,7 @@
         <v>1</v>
       </c>
       <c r="C123" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.45">
@@ -18701,7 +18742,7 @@
         <v>1</v>
       </c>
       <c r="C124" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.45">
@@ -18712,7 +18753,7 @@
         <v>1</v>
       </c>
       <c r="C125" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.45">
@@ -18723,7 +18764,7 @@
         <v>4</v>
       </c>
       <c r="C126" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.45">
@@ -18734,7 +18775,7 @@
         <v>8</v>
       </c>
       <c r="C127" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.45">
@@ -18745,7 +18786,7 @@
         <v>1</v>
       </c>
       <c r="C128" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.45">
@@ -18756,7 +18797,7 @@
         <v>1</v>
       </c>
       <c r="C129" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.45">
@@ -18767,7 +18808,7 @@
         <v>1</v>
       </c>
       <c r="C130" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.45">
@@ -18778,7 +18819,7 @@
         <v>1</v>
       </c>
       <c r="C131" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.45">
@@ -18789,7 +18830,7 @@
         <v>1</v>
       </c>
       <c r="C132" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.45">
@@ -18800,7 +18841,7 @@
         <v>1</v>
       </c>
       <c r="C133" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.45">
@@ -18811,7 +18852,7 @@
         <v>1</v>
       </c>
       <c r="C134" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.45">
@@ -18822,7 +18863,7 @@
         <v>2</v>
       </c>
       <c r="C135" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.45">
@@ -18833,7 +18874,7 @@
         <v>1</v>
       </c>
       <c r="C136" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.45">
@@ -18844,7 +18885,7 @@
         <v>1</v>
       </c>
       <c r="C137" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.45">
@@ -18855,7 +18896,7 @@
         <v>1</v>
       </c>
       <c r="C138" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.45">
@@ -18866,7 +18907,7 @@
         <v>2</v>
       </c>
       <c r="C139" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.45">
@@ -18877,7 +18918,7 @@
         <v>1</v>
       </c>
       <c r="C140" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.45">
@@ -18888,7 +18929,7 @@
         <v>1</v>
       </c>
       <c r="C141" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.45">
@@ -18899,7 +18940,7 @@
         <v>1</v>
       </c>
       <c r="C142" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.45">
@@ -18910,7 +18951,7 @@
         <v>2</v>
       </c>
       <c r="C143" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.45">
@@ -18921,7 +18962,7 @@
         <v>1</v>
       </c>
       <c r="C144" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.45">
@@ -18932,7 +18973,7 @@
         <v>2</v>
       </c>
       <c r="C145" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.45">
@@ -18943,7 +18984,7 @@
         <v>1</v>
       </c>
       <c r="C146" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.45">
@@ -18954,7 +18995,7 @@
         <v>1</v>
       </c>
       <c r="C147" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.45">
@@ -18965,7 +19006,7 @@
         <v>1</v>
       </c>
       <c r="C148" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.45">
@@ -18976,7 +19017,7 @@
         <v>1</v>
       </c>
       <c r="C149" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.45">
@@ -18987,7 +19028,7 @@
         <v>1</v>
       </c>
       <c r="C150" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.45">
@@ -18998,7 +19039,7 @@
         <v>1</v>
       </c>
       <c r="C151" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.45">
@@ -19009,7 +19050,7 @@
         <v>1</v>
       </c>
       <c r="C152" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.45">
@@ -19020,7 +19061,7 @@
         <v>1</v>
       </c>
       <c r="C153" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.45">
@@ -19031,7 +19072,7 @@
         <v>1</v>
       </c>
       <c r="C154" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.45">
@@ -19042,7 +19083,7 @@
         <v>1</v>
       </c>
       <c r="C155" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.45">
@@ -19053,7 +19094,7 @@
         <v>1</v>
       </c>
       <c r="C156" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.45">
@@ -19064,7 +19105,7 @@
         <v>1</v>
       </c>
       <c r="C157" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.45">
@@ -19075,7 +19116,7 @@
         <v>1</v>
       </c>
       <c r="C158" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.45">
@@ -19086,7 +19127,7 @@
         <v>1</v>
       </c>
       <c r="C159" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.45">
@@ -19097,7 +19138,7 @@
         <v>1</v>
       </c>
       <c r="C160" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.45">
@@ -19108,7 +19149,7 @@
         <v>1</v>
       </c>
       <c r="C161" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.45">
@@ -19119,7 +19160,7 @@
         <v>1</v>
       </c>
       <c r="C162" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.45">
@@ -19130,7 +19171,7 @@
         <v>1</v>
       </c>
       <c r="C163" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.45">
@@ -19141,7 +19182,7 @@
         <v>1</v>
       </c>
       <c r="C164" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.45">
@@ -19152,7 +19193,7 @@
         <v>1</v>
       </c>
       <c r="C165" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.45">
@@ -19163,7 +19204,7 @@
         <v>1</v>
       </c>
       <c r="C166" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.45">
@@ -19174,7 +19215,7 @@
         <v>2</v>
       </c>
       <c r="C167" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.45">
@@ -19185,7 +19226,7 @@
         <v>1</v>
       </c>
       <c r="C168" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.45">
@@ -19196,7 +19237,7 @@
         <v>1</v>
       </c>
       <c r="C169" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.45">
@@ -19207,7 +19248,7 @@
         <v>1</v>
       </c>
       <c r="C170" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.45">
@@ -19218,7 +19259,7 @@
         <v>1</v>
       </c>
       <c r="C171" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.45">
@@ -19229,7 +19270,7 @@
         <v>1</v>
       </c>
       <c r="C172" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.45">
@@ -19240,7 +19281,7 @@
         <v>1</v>
       </c>
       <c r="C173" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.45">
@@ -19251,7 +19292,7 @@
         <v>1</v>
       </c>
       <c r="C174" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.45">
@@ -19262,7 +19303,7 @@
         <v>1</v>
       </c>
       <c r="C175" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.45">
@@ -19273,7 +19314,7 @@
         <v>1</v>
       </c>
       <c r="C176" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.45">
@@ -19284,7 +19325,7 @@
         <v>1</v>
       </c>
       <c r="C177" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.45">
@@ -19295,7 +19336,7 @@
         <v>1</v>
       </c>
       <c r="C178" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.45">
@@ -19306,7 +19347,7 @@
         <v>1</v>
       </c>
       <c r="C179" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.45">
@@ -19317,7 +19358,7 @@
         <v>2</v>
       </c>
       <c r="C180" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.45">
@@ -19328,7 +19369,7 @@
         <v>1</v>
       </c>
       <c r="C181" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.45">
@@ -19339,7 +19380,7 @@
         <v>2</v>
       </c>
       <c r="C182" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.45">
@@ -19350,7 +19391,7 @@
         <v>1</v>
       </c>
       <c r="C183" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.45">
@@ -19361,7 +19402,7 @@
         <v>1</v>
       </c>
       <c r="C184" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.45">
@@ -19372,7 +19413,7 @@
         <v>1</v>
       </c>
       <c r="C185" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.45">
@@ -19383,7 +19424,7 @@
         <v>1</v>
       </c>
       <c r="C186" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.45">
@@ -19394,7 +19435,7 @@
         <v>1</v>
       </c>
       <c r="C187" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.45">
@@ -19405,7 +19446,7 @@
         <v>2</v>
       </c>
       <c r="C188" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.45">
@@ -19416,7 +19457,7 @@
         <v>1</v>
       </c>
       <c r="C189" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.45">
@@ -19427,7 +19468,7 @@
         <v>1</v>
       </c>
       <c r="C190" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.45">
@@ -19438,7 +19479,7 @@
         <v>1</v>
       </c>
       <c r="C191" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.45">
@@ -19449,7 +19490,7 @@
         <v>1</v>
       </c>
       <c r="C192" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.45">
@@ -19460,7 +19501,7 @@
         <v>2</v>
       </c>
       <c r="C193" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.45">
@@ -19471,7 +19512,7 @@
         <v>5</v>
       </c>
       <c r="C194" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.45">
@@ -19482,7 +19523,7 @@
         <v>1</v>
       </c>
       <c r="C195" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.45">
@@ -19493,7 +19534,7 @@
         <v>1</v>
       </c>
       <c r="C196" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.45">
@@ -19504,7 +19545,7 @@
         <v>1</v>
       </c>
       <c r="C197" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.45">
@@ -19515,7 +19556,7 @@
         <v>2</v>
       </c>
       <c r="C198" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.45">
@@ -19526,7 +19567,7 @@
         <v>1</v>
       </c>
       <c r="C199" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.45">
@@ -19537,7 +19578,7 @@
         <v>1</v>
       </c>
       <c r="C200" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.45">
@@ -19548,7 +19589,7 @@
         <v>2</v>
       </c>
       <c r="C201" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.45">
@@ -19559,7 +19600,7 @@
         <v>1</v>
       </c>
       <c r="C202" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.45">
@@ -19570,7 +19611,7 @@
         <v>2</v>
       </c>
       <c r="C203" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.45">
@@ -19581,7 +19622,7 @@
         <v>1</v>
       </c>
       <c r="C204" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.45">
@@ -19592,7 +19633,7 @@
         <v>1</v>
       </c>
       <c r="C205" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.45">
@@ -19603,7 +19644,7 @@
         <v>1</v>
       </c>
       <c r="C206" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.45">
@@ -19614,7 +19655,7 @@
         <v>1</v>
       </c>
       <c r="C207" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.45">
@@ -19625,7 +19666,7 @@
         <v>1</v>
       </c>
       <c r="C208" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.45">
@@ -19636,7 +19677,7 @@
         <v>1</v>
       </c>
       <c r="C209" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.45">
@@ -19647,7 +19688,7 @@
         <v>1</v>
       </c>
       <c r="C210" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.45">
@@ -19658,7 +19699,7 @@
         <v>1</v>
       </c>
       <c r="C211" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.45">
@@ -19669,7 +19710,7 @@
         <v>1</v>
       </c>
       <c r="C212" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.45">
@@ -19680,7 +19721,7 @@
         <v>2</v>
       </c>
       <c r="C213" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.45">
@@ -19691,7 +19732,7 @@
         <v>2</v>
       </c>
       <c r="C214" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.45">
@@ -19702,7 +19743,7 @@
         <v>1</v>
       </c>
       <c r="C215" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.45">
@@ -19713,7 +19754,7 @@
         <v>1</v>
       </c>
       <c r="C216" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.45">
@@ -19724,7 +19765,7 @@
         <v>1</v>
       </c>
       <c r="C217" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.45">
@@ -19735,7 +19776,7 @@
         <v>1</v>
       </c>
       <c r="C218" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.45">
@@ -19746,7 +19787,7 @@
         <v>1</v>
       </c>
       <c r="C219" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.45">
@@ -19757,7 +19798,7 @@
         <v>1</v>
       </c>
       <c r="C220" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.45">
@@ -19768,7 +19809,7 @@
         <v>1</v>
       </c>
       <c r="C221" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
improve abstract to use section
</commit_message>
<xml_diff>
--- a/scenario_tocs.xlsx
+++ b/scenario_tocs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\xMeta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF14D2DF-02B1-44D3-BF4A-C6DB2B452EB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F04D4AAC-012A-4898-A062-C034387CB130}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -5126,7 +5126,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{11E6CF5C-3969-4A20-9A1A-A3BC2CD2E22E}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{11E6CF5C-3969-4A20-9A1A-A3BC2CD2E22E}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B19" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="1">
     <pivotField axis="axisRow" dataField="1" showAll="0">
@@ -17093,7 +17093,7 @@
   <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17189,7 +17189,7 @@
         <v>1</v>
       </c>
       <c r="M2">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="N2" t="s">
         <v>14</v>
@@ -17230,7 +17230,7 @@
         <v>0</v>
       </c>
       <c r="M3">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="N3" t="s">
         <v>1530</v>
@@ -17271,7 +17271,7 @@
         <v>0</v>
       </c>
       <c r="M4">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="N4" t="s">
         <v>1530</v>
@@ -17303,7 +17303,7 @@
         <v>0</v>
       </c>
       <c r="J5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K5">
         <v>0</v>
@@ -17312,7 +17312,7 @@
         <v>0</v>
       </c>
       <c r="M5">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="N5" t="s">
         <v>1574</v>
@@ -17353,7 +17353,7 @@
         <v>0</v>
       </c>
       <c r="M6">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="N6" t="s">
         <v>929</v>
@@ -17394,7 +17394,7 @@
         <v>0</v>
       </c>
       <c r="M7">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="N7" t="s">
         <v>1092</v>
@@ -17435,7 +17435,7 @@
         <v>0</v>
       </c>
       <c r="M8">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="N8" t="s">
         <v>1530</v>
@@ -17476,7 +17476,7 @@
         <v>0</v>
       </c>
       <c r="M9">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="N9" t="s">
         <v>772</v>
@@ -17517,7 +17517,7 @@
         <v>0</v>
       </c>
       <c r="M10">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="N10" t="s">
         <v>489</v>
@@ -17558,7 +17558,7 @@
         <v>0</v>
       </c>
       <c r="M11">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="N11" t="s">
         <v>772</v>
@@ -17599,7 +17599,7 @@
         <v>0</v>
       </c>
       <c r="M12">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="N12" t="s">
         <v>212</v>

</xml_diff>